<commit_message>
English labels added to BDOT10k ontology
Signed-off-by: mereolog <pawel.garbacz@makolab.com>
</commit_message>
<xml_diff>
--- a/bdot10k_ontology/cellfie_import_data/BDOT_eng.xlsx
+++ b/bdot10k_ontology/cellfie_import_data/BDOT_eng.xlsx
@@ -152,7 +152,7 @@
     <t>road</t>
   </si>
   <si>
-    <t>auostrada</t>
+    <t>autostrada</t>
   </si>
   <si>
     <t>highway</t>
@@ -422,13 +422,13 @@
     <t>one-family housing</t>
   </si>
   <si>
-    <t>zabudowa przemysłowo-składowa</t>
+    <t>zabudowa przemysłowo‐składowa</t>
   </si>
   <si>
     <t>industrial and warehouse buildings</t>
   </si>
   <si>
-    <t>zabudowa handlowo-usługowa</t>
+    <t>zabudowa handlowo‐usługowa</t>
   </si>
   <si>
     <t>commercial and service buildings</t>
@@ -587,7 +587,7 @@
     <t>sandy or gravel ground</t>
   </si>
   <si>
-    <t>pozostały grunt nieużytkowy</t>
+    <t>pozostały grunt nieużytkowany</t>
   </si>
   <si>
     <t>the remaining unused land</t>
@@ -647,7 +647,7 @@
     <t>area under technical or construction equipment</t>
   </si>
   <si>
-    <t>teren przemysłowo-składowy</t>
+    <t>teren przemysłowo‐składowy</t>
   </si>
   <si>
     <t>industrial and storage area</t>
@@ -695,7 +695,7 @@
     <t>hotel buildings</t>
   </si>
   <si>
-    <t>budynki zakwaterowania turystycznego, pozostałe</t>
+    <t>budynki zakwaterowania turystycznego,pozostałe</t>
   </si>
   <si>
     <t>tourist accommodation buildings, others</t>
@@ -770,7 +770,7 @@
     <t>farm buildings</t>
   </si>
   <si>
-    <t>budynki przeznaczone do sprawowania kultur religijnego i czynności religijnych</t>
+    <t>budynki przeznaczone do sprawowania kultu religijnego i czynności religijnych</t>
   </si>
   <si>
     <t>buildings intended for religious worship and religious activities</t>
@@ -935,7 +935,7 @@
     <t>artificial slope</t>
   </si>
   <si>
-    <t>tor sachochodowy</t>
+    <t>tor samochodowy</t>
   </si>
   <si>
     <t>car track</t>
@@ -980,7 +980,7 @@
     <t>maszt telekomunikacyjny</t>
   </si>
   <si>
-    <t>telecommunications mast</t>
+    <t>telecommunication mast</t>
   </si>
   <si>
     <t>turbina wiatrowa</t>
@@ -989,7 +989,7 @@
     <t>wind turbine</t>
   </si>
   <si>
-    <t>slup energetyczny</t>
+    <t>słup energetyczny</t>
   </si>
   <si>
     <t>power pole</t>
@@ -1187,7 +1187,7 @@
     <t>set of fuel dispensers</t>
   </si>
   <si>
-    <t>zespół urządzeń stacji metereologicznej</t>
+    <t>zespół urządzeń stacji meteorologicznej</t>
   </si>
   <si>
     <t>set of devices of the meteorological station</t>
@@ -1313,7 +1313,7 @@
     <t>ironworks</t>
   </si>
   <si>
-    <t>koplania</t>
+    <t>kopalnia</t>
   </si>
   <si>
     <t>mine</t>
@@ -1382,7 +1382,8 @@
     <t>commercial and service complex</t>
   </si>
   <si>
-    <t>centrum handlowo-usługowe</t>
+    <t xml:space="preserve">centrum handlowo‐usługowe
+</t>
   </si>
   <si>
     <t>commercial and service centre</t>
@@ -1478,7 +1479,7 @@
     <t>zoological garden</t>
   </si>
   <si>
-    <t>ośrodek sportowo-rekreacyjny</t>
+    <t>ośrodek sportowo‐rekreacyjny</t>
   </si>
   <si>
     <t>sports and recreational centre</t>
@@ -1529,7 +1530,7 @@
     <t>educational complex</t>
   </si>
   <si>
-    <t>ośrodek naukowo-badawczy</t>
+    <t>ośrodek naukowo‐badawczy</t>
   </si>
   <si>
     <t>research and development center</t>
@@ -1589,7 +1590,7 @@
     <t>open-air museum</t>
   </si>
   <si>
-    <t>twierdza nad forteca</t>
+    <t>twierdza lub forteca</t>
   </si>
   <si>
     <t>fortress</t>
@@ -1721,19 +1722,19 @@
     <t>rural commune</t>
   </si>
   <si>
-    <t>gmina miejsko-wiejska</t>
+    <t>gmina miejsko‐wiejska</t>
   </si>
   <si>
     <t>municipal-rural commune</t>
   </si>
   <si>
-    <t>miasto w gminie miejsko-wiejskiej</t>
+    <t>miasto w gminie miejsko‐wiejskiej</t>
   </si>
   <si>
     <t>town in a municipal-rural commune</t>
   </si>
   <si>
-    <t>obszar wiejski w gminie miejsko-wiejskiej</t>
+    <t>obszar wiejski w gminie miejsko‐wiejskiej</t>
   </si>
   <si>
     <t>rural area in a municipal-rural commune</t>
@@ -2109,10 +2110,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -2137,7 +2142,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -3363,7 +3368,7 @@
       <c r="D50" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="3" t="s">
         <v>134</v>
       </c>
       <c r="F50" s="1" t="s">
@@ -3383,7 +3388,7 @@
       <c r="D51" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="3" t="s">
         <v>136</v>
       </c>
       <c r="F51" s="1" t="s">
@@ -3803,7 +3808,7 @@
       <c r="D72" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="3" t="s">
         <v>189</v>
       </c>
       <c r="F72" s="1" t="s">
@@ -3943,7 +3948,7 @@
       <c r="D79" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>209</v>
       </c>
       <c r="F79" s="1" t="s">
@@ -4803,7 +4808,7 @@
       <c r="D122" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E122" s="3" t="s">
         <v>305</v>
       </c>
       <c r="F122" s="1" t="s">
@@ -4926,7 +4931,7 @@
       <c r="E128" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F128" s="2" t="s">
         <v>320</v>
       </c>
     </row>
@@ -4963,7 +4968,7 @@
       <c r="D130" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="E130" s="3" t="s">
         <v>323</v>
       </c>
       <c r="F130" s="2" t="s">
@@ -5523,7 +5528,7 @@
       <c r="D158" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E158" s="2" t="s">
+      <c r="E158" s="3" t="s">
         <v>389</v>
       </c>
       <c r="F158" s="1" t="s">
@@ -5603,7 +5608,7 @@
       <c r="D162" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="E162" s="3" t="s">
+      <c r="E162" s="4" t="s">
         <v>401</v>
       </c>
       <c r="F162" s="1" t="s">
@@ -6343,7 +6348,7 @@
       <c r="D199" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="E199" s="2" t="s">
+      <c r="E199" s="3" t="s">
         <v>486</v>
       </c>
       <c r="F199" s="1" t="s">
@@ -6483,7 +6488,7 @@
       <c r="D206" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E206" s="2" t="s">
+      <c r="E206" s="3" t="s">
         <v>503</v>
       </c>
       <c r="F206" s="1" t="s">
@@ -6643,7 +6648,7 @@
       <c r="D214" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="E214" s="2" t="s">
+      <c r="E214" s="3" t="s">
         <v>523</v>
       </c>
       <c r="F214" s="1" t="s">
@@ -6979,7 +6984,7 @@
       <c r="D231" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="E231" s="2" t="s">
+      <c r="E231" s="3" t="s">
         <v>567</v>
       </c>
       <c r="F231" s="1" t="s">
@@ -6999,7 +7004,7 @@
       <c r="D232" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="E232" s="2" t="s">
+      <c r="E232" s="3" t="s">
         <v>569</v>
       </c>
       <c r="F232" s="1" t="s">
@@ -7019,7 +7024,7 @@
       <c r="D233" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="E233" s="2" t="s">
+      <c r="E233" s="3" t="s">
         <v>571</v>
       </c>
       <c r="F233" s="1" t="s">

</xml_diff>